<commit_message>
enhnacements in call_queue monitoring
</commit_message>
<xml_diff>
--- a/Appointment_Details.xlsx
+++ b/Appointment_Details.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,100 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Aarav Mehta</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>morning</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>डॉ. से</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>917823844614</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>24 MG Road, Bengaluru</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2025-06-25 18:43:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Aarav Mehta</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>morning</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>डॉ. से</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>917823844614</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>24 MG Road, Bengaluru</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2025-06-25 19:32:35</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>